<commit_message>
Anpassung IPE Tabelle und Auswahl der Profile
</commit_message>
<xml_diff>
--- a/tabellen/Tabelle_IPE.xlsx
+++ b/tabellen/Tabelle_IPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\OneDrive\Desktop\projectbeaverdam\Bachelorarbeit B4 Trako Joel Manolias 406534\Code_B_T\tabellen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelm\OneDrive\Desktop\Dokumentation\10.1.2024\tabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3721C28-9270-4874-B31D-32AA420E2F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939456BC-3939-4E43-928A-80476E577969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{DA9B8BCA-C3F0-4356-8462-02321319B5F9}"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="25580" windowHeight="13660" xr2:uid="{DA9B8BCA-C3F0-4356-8462-02321319B5F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
   <si>
     <t>h</t>
   </si>
@@ -80,36 +80,18 @@
     <t>146</t>
   </si>
   <si>
-    <t>1510</t>
-  </si>
-  <si>
-    <t>165</t>
-  </si>
-  <si>
     <t>1940</t>
   </si>
   <si>
     <t>194</t>
   </si>
   <si>
-    <t>2210</t>
-  </si>
-  <si>
-    <t>219</t>
-  </si>
-  <si>
     <t>2770</t>
   </si>
   <si>
     <t>252</t>
   </si>
   <si>
-    <t>3130</t>
-  </si>
-  <si>
-    <t>282</t>
-  </si>
-  <si>
     <t>30.7</t>
   </si>
   <si>
@@ -119,96 +101,42 @@
     <t>324</t>
   </si>
   <si>
-    <t>4370</t>
-  </si>
-  <si>
-    <t>361</t>
-  </si>
-  <si>
     <t>5790</t>
   </si>
   <si>
     <t>429</t>
   </si>
   <si>
-    <t>6950</t>
-  </si>
-  <si>
-    <t>507</t>
-  </si>
-  <si>
     <t>8360</t>
   </si>
   <si>
     <t>557</t>
   </si>
   <si>
-    <t>9990</t>
-  </si>
-  <si>
-    <t>658</t>
-  </si>
-  <si>
     <t>11770</t>
   </si>
   <si>
     <t>713</t>
   </si>
   <si>
-    <t>13910</t>
-  </si>
-  <si>
-    <t>833</t>
-  </si>
-  <si>
     <t>16270</t>
   </si>
   <si>
     <t>904</t>
   </si>
   <si>
-    <t>19050</t>
-  </si>
-  <si>
-    <t>1050</t>
-  </si>
-  <si>
     <t>23130</t>
   </si>
   <si>
     <t>1160</t>
   </si>
   <si>
-    <t>26750</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>840</t>
-  </si>
-  <si>
-    <t>30120</t>
-  </si>
-  <si>
-    <t>1480</t>
-  </si>
-  <si>
     <t>33740</t>
   </si>
   <si>
     <t>1500</t>
   </si>
   <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>40920</t>
-  </si>
-  <si>
-    <t>1790</t>
-  </si>
-  <si>
     <t>132</t>
   </si>
   <si>
@@ -230,27 +158,6 @@
     <t>1930</t>
   </si>
   <si>
-    <t>137</t>
-  </si>
-  <si>
-    <t>57580</t>
-  </si>
-  <si>
-    <t>2280</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>70720</t>
-  </si>
-  <si>
-    <t>2750</t>
-  </si>
-  <si>
     <t>134</t>
   </si>
   <si>
@@ -266,27 +173,6 @@
     <t>156</t>
   </si>
   <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>79160</t>
-  </si>
-  <si>
-    <t>2850</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>102300</t>
-  </si>
-  <si>
-    <t>3620</t>
-  </si>
-  <si>
     <t>122</t>
   </si>
   <si>
@@ -296,30 +182,6 @@
     <t>3070</t>
   </si>
   <si>
-    <t>197</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
-    <t>118300</t>
-  </si>
-  <si>
-    <t>3880</t>
-  </si>
-  <si>
-    <t>234</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>141600</t>
-  </si>
-  <si>
-    <t>4580</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
@@ -335,24 +197,12 @@
     <t>77.3</t>
   </si>
   <si>
-    <t>32.0</t>
-  </si>
-  <si>
     <t>33.4</t>
   </si>
   <si>
-    <t>37.4</t>
-  </si>
-  <si>
     <t>39.1</t>
   </si>
   <si>
-    <t>43.7</t>
-  </si>
-  <si>
-    <t>34.3</t>
-  </si>
-  <si>
     <t>45.9</t>
   </si>
   <si>
@@ -362,102 +212,39 @@
     <t>53.8</t>
   </si>
   <si>
-    <t>42.3</t>
-  </si>
-  <si>
     <t>42.2</t>
   </si>
   <si>
-    <t>62.8</t>
-  </si>
-  <si>
-    <t>49.3</t>
-  </si>
-  <si>
     <t>62.6</t>
   </si>
   <si>
     <t>49.1</t>
   </si>
   <si>
-    <t>72.6</t>
-  </si>
-  <si>
-    <t>57.0</t>
-  </si>
-  <si>
     <t>72.7</t>
   </si>
   <si>
     <t>57.1</t>
   </si>
   <si>
-    <t>36.4</t>
-  </si>
-  <si>
-    <t>84.1</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
     <t>84.5</t>
   </si>
   <si>
     <t>66.3</t>
   </si>
   <si>
-    <t>40.4</t>
-  </si>
-  <si>
-    <t>96.4</t>
-  </si>
-  <si>
-    <t>75.7</t>
-  </si>
-  <si>
-    <t>40.8</t>
-  </si>
-  <si>
     <t>98.8</t>
   </si>
   <si>
     <t>77.6</t>
   </si>
   <si>
-    <t>45.6</t>
-  </si>
-  <si>
-    <t>92.4</t>
-  </si>
-  <si>
     <t>90.7</t>
   </si>
   <si>
-    <t>50.6</t>
-  </si>
-  <si>
-    <t>51.4</t>
-  </si>
-  <si>
-    <t>55.6</t>
-  </si>
-  <si>
-    <t>56.6</t>
-  </si>
-  <si>
-    <t>61.8</t>
-  </si>
-  <si>
-    <t>22.8</t>
-  </si>
-  <si>
     <t>22.4</t>
   </si>
   <si>
-    <t>21.6</t>
-  </si>
-  <si>
     <t>7.6</t>
   </si>
   <si>
@@ -476,30 +263,9 @@
     <t>23.9</t>
   </si>
   <si>
-    <t>27.1</t>
-  </si>
-  <si>
     <t>28.5</t>
   </si>
   <si>
-    <t>18.2</t>
-  </si>
-  <si>
-    <t>20.2</t>
-  </si>
-  <si>
-    <t>22.2</t>
-  </si>
-  <si>
-    <t>24.2</t>
-  </si>
-  <si>
-    <t>27.4</t>
-  </si>
-  <si>
-    <t>30.4</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -551,18 +317,6 @@
     <t>18.8</t>
   </si>
   <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>21.3</t>
-  </si>
-  <si>
-    <t>10.2</t>
-  </si>
-  <si>
-    <t>25.1</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -572,51 +326,30 @@
     <t>26.2</t>
   </si>
   <si>
-    <t>11.2</t>
-  </si>
-  <si>
-    <t>29.4</t>
-  </si>
-  <si>
     <t>24</t>
   </si>
   <si>
-    <t>12.2</t>
-  </si>
-  <si>
     <t>27</t>
   </si>
   <si>
     <t>13.5</t>
   </si>
   <si>
-    <t>13.6</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
     <t>15</t>
   </si>
   <si>
-    <t>15.2</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
-    <t>16.2</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>17.2</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
@@ -626,9 +359,6 @@
     <t>19</t>
   </si>
   <si>
-    <t>19.2</t>
-  </si>
-  <si>
     <t>46</t>
   </si>
   <si>
@@ -638,22 +368,13 @@
     <t>50</t>
   </si>
   <si>
-    <t>20.4</t>
-  </si>
-  <si>
     <t>55</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>21.2</t>
-  </si>
-  <si>
     <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64033E-3135-4086-AA7F-7654CF20D009}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,22 +776,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="G2" s="1"/>
       <c r="I2" s="1"/>
@@ -1078,22 +799,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1"/>
       <c r="I3" s="1"/>
@@ -1101,22 +822,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1"/>
       <c r="I4" s="1"/>
@@ -1124,22 +845,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1"/>
       <c r="I5" s="1"/>
@@ -1147,16 +868,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>167</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1170,16 +891,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1193,16 +914,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1216,16 +937,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>147</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -1239,22 +960,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1"/>
       <c r="I10" s="1"/>
@@ -1262,22 +983,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>
@@ -1285,22 +1006,22 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>179</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="1"/>
@@ -1308,16 +1029,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>180</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
@@ -1331,16 +1052,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -1354,16 +1075,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>90</v>
       </c>
       <c r="B15" t="s">
-        <v>182</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -1377,16 +1098,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>31</v>
@@ -1400,22 +1121,22 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G17" s="1"/>
       <c r="I17" s="1"/>
@@ -1423,22 +1144,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G18" s="1"/>
       <c r="I18" s="1"/>
@@ -1446,22 +1167,22 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G19" s="1"/>
       <c r="I19" s="1"/>
@@ -1469,414 +1190,108 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F20" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B21" t="s">
-        <v>190</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" t="s">
-        <v>42</v>
-      </c>
       <c r="G21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
       <c r="G22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>168</v>
-      </c>
-      <c r="B23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" t="s">
-        <v>46</v>
-      </c>
       <c r="G23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
       <c r="G24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
-      <c r="F25" t="s">
-        <v>51</v>
-      </c>
       <c r="G25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" t="s">
-        <v>194</v>
-      </c>
-      <c r="C26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" t="s">
-        <v>53</v>
-      </c>
       <c r="G26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" t="s">
-        <v>56</v>
-      </c>
       <c r="G27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B28" t="s">
-        <v>197</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" t="s">
-        <v>60</v>
-      </c>
       <c r="G28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" t="s">
-        <v>199</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
       <c r="G29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>149</v>
-      </c>
-      <c r="B30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" t="s">
-        <v>66</v>
-      </c>
       <c r="G30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>200</v>
-      </c>
-      <c r="B31" t="s">
-        <v>133</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" t="s">
-        <v>70</v>
-      </c>
       <c r="G31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>202</v>
-      </c>
-      <c r="B32" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" t="s">
-        <v>73</v>
-      </c>
-      <c r="F32" t="s">
-        <v>74</v>
-      </c>
       <c r="G32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>203</v>
-      </c>
-      <c r="B33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" t="s">
-        <v>78</v>
-      </c>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>139</v>
-      </c>
-      <c r="B34" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" t="s">
-        <v>82</v>
-      </c>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="B35" t="s">
-        <v>204</v>
-      </c>
-      <c r="C35" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" t="s">
-        <v>85</v>
-      </c>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" t="s">
-        <v>205</v>
-      </c>
-      <c r="C36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" t="s">
-        <v>88</v>
-      </c>
-      <c r="F36" t="s">
-        <v>89</v>
-      </c>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C37" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" t="s">
-        <v>93</v>
-      </c>
+    <row r="37" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>

</xml_diff>